<commit_message>
Removed old file, replaced with updated named file
</commit_message>
<xml_diff>
--- a/fitness/2023/08/2023_GymJournal.xlsx
+++ b/fitness/2023/08/2023_GymJournal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmorgan\Desktop\1%Better\Fitness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\morganbo85\fitness\2023\08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0988DF-8574-4335-922F-AF19FA164EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A09400-FE5C-494B-AF18-18AD155A4DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFC2F964-F086-4AE0-9862-6E288B172C16}"/>
   </bookViews>
@@ -172,13 +172,13 @@
     <t>Decline Sit Ups</t>
   </si>
   <si>
-    <t>Week 5 Day #######</t>
-  </si>
-  <si>
     <t>Week 5 Day 2: ########</t>
   </si>
   <si>
     <t>Week 5 Day 3: ###########</t>
+  </si>
+  <si>
+    <t>Week 5 Day 08/20/2023</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -363,6 +363,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -379,27 +397,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -751,58 +748,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="16" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="19" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="19" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="26" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1746,14 +1743,14 @@
       <c r="J26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="5">
         <v>130</v>
       </c>
       <c r="L26" s="6">
         <v>8</v>
       </c>
       <c r="M26" s="4"/>
-      <c r="N26" s="22"/>
+      <c r="N26" s="5"/>
       <c r="O26" s="6">
         <v>15</v>
       </c>
@@ -1789,14 +1786,14 @@
       <c r="J27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="5">
         <v>130</v>
       </c>
       <c r="L27" s="6">
         <v>8</v>
       </c>
       <c r="M27" s="4"/>
-      <c r="N27" s="22"/>
+      <c r="N27" s="5"/>
       <c r="O27" s="6">
         <v>15</v>
       </c>
@@ -1851,7 +1848,7 @@
       <c r="M30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N30" s="22">
+      <c r="N30" s="5">
         <v>130</v>
       </c>
       <c r="O30" s="6">
@@ -1862,7 +1859,7 @@
       <c r="M31" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N31" s="22">
+      <c r="N31" s="5">
         <v>130</v>
       </c>
       <c r="O31" s="6">
@@ -1923,58 +1920,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="16" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
+      <c r="A2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="20"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -3178,58 +3175,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="16" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="19" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="19" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="29" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -4429,6 +4426,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f46d2067-2890-4ae8-8452-93928e3b4319" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084F2CDD4EF4E5B418A98476F1A4DAA70" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ffd2ce33271a21beae77e6fbef18e9f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f46d2067-2890-4ae8-8452-93928e3b4319" xmlns:ns4="d2ed02d4-8f5a-483b-a9ee-c01ec23f1fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ae291de4fe85ad6ed2f8f8c4dff21cb" ns3:_="" ns4:_="">
     <xsd:import namespace="f46d2067-2890-4ae8-8452-93928e3b4319"/>
@@ -4657,24 +4671,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1AFCF62-3E01-4379-92B9-3727E2696821}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d2ed02d4-8f5a-483b-a9ee-c01ec23f1fcd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f46d2067-2890-4ae8-8452-93928e3b4319"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f46d2067-2890-4ae8-8452-93928e3b4319" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7387E2AA-A38A-4B2E-B41D-563EEEA3DD39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7089663E-E8F1-44A4-A1A6-E75F5CE9D79B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4691,29 +4713,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7387E2AA-A38A-4B2E-B41D-563EEEA3DD39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1AFCF62-3E01-4379-92B9-3727E2696821}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d2ed02d4-8f5a-483b-a9ee-c01ec23f1fcd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f46d2067-2890-4ae8-8452-93928e3b4319"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>